<commit_message>
Corma: battery measurement added.
</commit_message>
<xml_diff>
--- a/Corma/Corma.xlsx
+++ b/Corma/Corma.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="19080" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Timer f in</t>
   </si>
@@ -55,6 +55,30 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Pkt Dur</t>
+  </si>
+  <si>
+    <t>Cycle duration</t>
+  </si>
+  <si>
+    <t>Uref</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>1 bit</t>
+  </si>
+  <si>
+    <t>Uin</t>
+  </si>
+  <si>
+    <t>UinADC</t>
+  </si>
+  <si>
+    <t>ADC out</t>
   </si>
 </sst>
 </file>
@@ -179,12 +203,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -490,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,8 +526,8 @@
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -513,7 +538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -521,7 +546,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,7 +558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -545,12 +570,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -559,39 +584,122 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4">
         <f>B7*1000/B5</f>
-        <v>328.125</v>
+        <v>531.25</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>23*1.5</f>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>329</v>
+      <c r="B10" s="2">
+        <v>5040</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <f>B10*B5/1000</f>
-        <v>21.056000000000001</v>
+        <v>322.56</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <f xml:space="preserve"> 1.1*B10*10</f>
+        <v>55440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <f>B13*B5/1000</f>
+        <v>3548.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2560</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <f>B17/1024</f>
+        <v>2.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3600</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <f>B19/2</f>
+        <v>1800</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
+        <f>B20/B18</f>
+        <v>720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>